<commit_message>
included pedestrians on priority formula
</commit_message>
<xml_diff>
--- a/docs/Fórmulas-polinomiais-excel.xlsx
+++ b/docs/Fórmulas-polinomiais-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtorres\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rtorres\eclipse-workspace\AIAD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83DEFF86-3BEE-4D8F-8D27-1EBA18A62791}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D31D4C-4CC3-48EF-AD55-390CA2931848}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{5DF59861-CD3F-4726-9ACC-EDA114ED9898}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{5DF59861-CD3F-4726-9ACC-EDA114ED9898}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Tempo desligado graph</t>
+  </si>
+  <si>
+    <t>Tempo aceso graph</t>
+  </si>
+  <si>
+    <t>Carros graph (não utilizado)</t>
   </si>
 </sst>
 </file>
@@ -214,46 +223,48 @@
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Folha1!$A$2:$A$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>0,1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2</c:v>
+                  <c:v>0,2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0,3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4</c:v>
+                  <c:v>0,4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>0,5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.6</c:v>
+                  <c:v>0,6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7</c:v>
+                  <c:v>0,7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79999999999999993</c:v>
+                  <c:v>0,8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.89999999999999991</c:v>
+                  <c:v>0,9</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="15">
+                  <c:v>Tempo aceso graph</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -265,34 +276,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>3.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -636,7 +647,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.8</c:v>
@@ -957,59 +968,65 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Folha1!$A$34:$A$50</c:f>
+              <c:f>Folha1!$A$44:$A$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>130</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>140</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>160</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>170</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>180</c:v>
                 </c:pt>
               </c:numCache>
@@ -1017,60 +1034,66 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$B$34:$B$50</c:f>
+              <c:f>Folha1!$B$44:$B$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.9</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1.6</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>2.4</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>3.3</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>3.8</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>4.4000000000000004</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>4.9000000000000004</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>5</c:v>
+                <c:pt idx="17">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1269,6 +1292,464 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-PT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Folha1!$A$65:$A$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Folha1!$B$65:$B$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.38</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.43</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.48</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.54</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.66</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.73</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.79</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.86</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.93</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F133-4E3B-A275-D16A2B116B84}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="475110152"/>
+        <c:axId val="475108512"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="475110152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="475108512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="475108512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="475110152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1389,6 +1870,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2422,6 +2943,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3042,6 +4079,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6F0C823-30A3-4735-B260-654A2CBA5174}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3347,10 +4420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E9022D-30B9-40E6-9E52-14CAEFCC8915}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3381,7 +4454,10 @@
         <v>0.1</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>0.6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3390,7 +4466,7 @@
         <v>0.2</v>
       </c>
       <c r="B4">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3399,7 +4475,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B5">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3408,7 +4484,7 @@
         <v>0.4</v>
       </c>
       <c r="B6">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3417,7 +4493,7 @@
         <v>0.5</v>
       </c>
       <c r="B7">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3426,7 +4502,7 @@
         <v>0.6</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3435,7 +4511,7 @@
         <v>0.7</v>
       </c>
       <c r="B9">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3444,7 +4520,7 @@
         <v>0.79999999999999993</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3453,7 +4529,7 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3461,10 +4537,14 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>0</v>
@@ -3480,7 +4560,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="2">
-        <v>5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3563,154 +4643,375 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <v>20</v>
-      </c>
-      <c r="B34" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>30</v>
-      </c>
-      <c r="B35">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>40</v>
-      </c>
-      <c r="B36">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>50</v>
-      </c>
-      <c r="B37">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>60</v>
-      </c>
-      <c r="B38">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>70</v>
-      </c>
-      <c r="B39">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>80</v>
-      </c>
-      <c r="B40">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>90</v>
-      </c>
-      <c r="B41">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>100</v>
-      </c>
-      <c r="B42">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>110</v>
-      </c>
-      <c r="B43">
-        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="B44">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45">
-        <f>A44+10</f>
-        <v>130</v>
+        <v>10</v>
       </c>
       <c r="B45">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <f t="shared" ref="A46:A49" si="1">A45+10</f>
-        <v>140</v>
-      </c>
-      <c r="B46">
-        <v>3.3</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>20</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="1"/>
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="B47">
-        <v>3.8</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
+        <v>40</v>
+      </c>
+      <c r="B48">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>50</v>
+      </c>
+      <c r="B49">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>60</v>
+      </c>
+      <c r="B50">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>70</v>
+      </c>
+      <c r="B51">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>80</v>
+      </c>
+      <c r="B52">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>90</v>
+      </c>
+      <c r="B53">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>100</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>110</v>
+      </c>
+      <c r="B55">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>120</v>
+      </c>
+      <c r="B56">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f>A56+10</f>
+        <v>130</v>
+      </c>
+      <c r="B57">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f>A57+10</f>
+        <v>140</v>
+      </c>
+      <c r="B58">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f>A58+10</f>
+        <v>150</v>
+      </c>
+      <c r="B59">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f>A59+10</f>
+        <v>160</v>
+      </c>
+      <c r="B60">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <f>A60+10</f>
+        <v>170</v>
+      </c>
+      <c r="B61">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>180</v>
+      </c>
+      <c r="B62" s="2">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>0</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f>A65+1</f>
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" ref="A67:A85" si="1">A66+1</f>
+        <v>2</v>
+      </c>
+      <c r="B67">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
         <f t="shared" si="1"/>
-        <v>160</v>
-      </c>
-      <c r="B48">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
         <f t="shared" si="1"/>
-        <v>170</v>
-      </c>
-      <c r="B49">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <v>180</v>
-      </c>
-      <c r="B50" s="2">
+        <v>4</v>
+      </c>
+      <c r="B69">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="1"/>
         <v>5</v>
+      </c>
+      <c r="B70">
+        <v>-0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B71">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B72">
+        <v>-0.23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B73">
+        <v>-0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B74">
+        <v>-0.34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B75">
+        <v>-0.38</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B76">
+        <f>-0.43</f>
+        <v>-0.43</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B77">
+        <v>-0.48</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B78">
+        <v>-0.54</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B79">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <f>A79+1</f>
+        <v>15</v>
+      </c>
+      <c r="B80">
+        <f>-0.66</f>
+        <v>-0.66</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B81">
+        <f>-0.73</f>
+        <v>-0.73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B82">
+        <f>-0.79</f>
+        <v>-0.79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B83">
+        <f>-0.86</f>
+        <v>-0.86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <f>A83+1</f>
+        <v>19</v>
+      </c>
+      <c r="B84">
+        <v>-0.93</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B85">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>